<commit_message>
start the game, exposed main picture(temporary)
</commit_message>
<xml_diff>
--- a/user_stories.xlsx
+++ b/user_stories.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="1280" yWindow="460" windowWidth="24340" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="User Stories" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="80">
   <si>
     <t>Role 
 "As a"</t>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>am on round 16</t>
+  </si>
+  <si>
+    <t>Built</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -436,7 +442,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -446,9 +452,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -474,20 +477,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -772,49 +781,49 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:A24"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="5" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
     <col min="4" max="4" width="46.83203125" customWidth="1"/>
     <col min="5" max="5" width="51.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="20" customWidth="1"/>
+    <col min="7" max="7" width="8" style="20" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -829,12 +838,16 @@
       <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="F2" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
+      <c r="A3" s="15"/>
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -847,12 +860,18 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
+      <c r="F3" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I4" s="8"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
@@ -867,9 +886,15 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
+      <c r="F5" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="16"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -884,7 +909,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B8" t="s">
@@ -901,7 +926,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -916,7 +941,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B11" t="s">
@@ -933,11 +958,11 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
+      <c r="A12" s="18"/>
       <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D12" t="s">
@@ -948,7 +973,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
+      <c r="A13" s="18"/>
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -963,7 +988,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
+      <c r="A14" s="18"/>
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -978,7 +1003,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
@@ -995,7 +1020,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
+      <c r="A17" s="18"/>
       <c r="B17" t="s">
         <v>34</v>
       </c>
@@ -1010,7 +1035,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
+      <c r="A18" s="18"/>
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -1025,22 +1050,22 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
-      <c r="B19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="A19" s="18"/>
+      <c r="B19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="18" t="s">
         <v>48</v>
       </c>
       <c r="B21" t="s">
@@ -1057,14 +1082,14 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="16"/>
+      <c r="A22" s="18"/>
       <c r="B22" t="s">
         <v>45</v>
       </c>
       <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E22" t="s">
@@ -1072,7 +1097,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
+      <c r="A23" s="18"/>
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -1087,22 +1112,22 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
-      <c r="B24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="7" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="18" t="s">
         <v>53</v>
       </c>
       <c r="B26" t="s">
@@ -1119,7 +1144,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="16"/>
+      <c r="A27" s="18"/>
       <c r="B27" t="s">
         <v>34</v>
       </c>
@@ -1134,7 +1159,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="16"/>
+      <c r="A28" s="18"/>
       <c r="B28" t="s">
         <v>34</v>
       </c>
@@ -1149,22 +1174,22 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
-      <c r="B29" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="A29" s="18"/>
+      <c r="B29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="18" t="s">
         <v>59</v>
       </c>
       <c r="B31" t="s">
@@ -1181,7 +1206,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="16"/>
+      <c r="A32" s="18"/>
       <c r="B32" t="s">
         <v>34</v>
       </c>
@@ -1196,7 +1221,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="16"/>
+      <c r="A33" s="18"/>
       <c r="B33" t="s">
         <v>34</v>
       </c>
@@ -1211,22 +1236,22 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
-      <c r="B34" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="7" t="s">
+      <c r="A34" s="18"/>
+      <c r="B34" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="18" t="s">
         <v>63</v>
       </c>
       <c r="B36" t="s">
@@ -1243,7 +1268,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="16"/>
+      <c r="A37" s="18"/>
       <c r="B37" t="s">
         <v>45</v>
       </c>
@@ -1258,7 +1283,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="16"/>
+      <c r="A38" s="18"/>
       <c r="B38" t="s">
         <v>34</v>
       </c>
@@ -1273,22 +1298,22 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="16"/>
-      <c r="B39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="7" t="s">
+      <c r="A39" s="18"/>
+      <c r="B39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="17" t="s">
         <v>64</v>
       </c>
       <c r="B41" t="s">
@@ -1305,7 +1330,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="15"/>
+      <c r="A42" s="17"/>
       <c r="B42" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
first round: added head options and check correct head function
</commit_message>
<xml_diff>
--- a/user_stories.xlsx
+++ b/user_stories.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="460" windowWidth="24340" windowHeight="14280" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="1260" yWindow="460" windowWidth="24340" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="81">
   <si>
     <t>Role 
 "As a"</t>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Built (temp)</t>
   </si>
 </sst>
 </file>
@@ -323,7 +326,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +336,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,7 +451,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,6 +486,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -492,10 +507,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -781,7 +794,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,9 +804,9 @@
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
     <col min="4" max="4" width="46.83203125" customWidth="1"/>
     <col min="5" max="5" width="51.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="20" customWidth="1"/>
-    <col min="7" max="7" width="8" style="20" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="15" customWidth="1"/>
+    <col min="7" max="7" width="8" style="15" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
@@ -823,7 +836,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -838,16 +851,16 @@
       <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
+      <c r="A3" s="17"/>
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -860,10 +873,10 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="15" t="s">
         <v>79</v>
       </c>
     </row>
@@ -871,7 +884,7 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
@@ -886,15 +899,15 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="15" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -907,26 +920,37 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="F6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="F8" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
+      <c r="A9" s="19"/>
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -939,9 +963,15 @@
       <c r="E9" t="s">
         <v>24</v>
       </c>
+      <c r="F9" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B11" t="s">
@@ -958,7 +988,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
+      <c r="A12" s="20"/>
       <c r="B12" t="s">
         <v>34</v>
       </c>
@@ -973,7 +1003,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
+      <c r="A13" s="20"/>
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -988,7 +1018,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
+      <c r="A14" s="20"/>
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -1003,7 +1033,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
@@ -1020,7 +1050,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
+      <c r="A17" s="20"/>
       <c r="B17" t="s">
         <v>34</v>
       </c>
@@ -1035,7 +1065,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
+      <c r="A18" s="20"/>
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -1050,7 +1080,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="6" t="s">
         <v>9</v>
       </c>
@@ -1065,7 +1095,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B21" t="s">
@@ -1082,7 +1112,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
+      <c r="A22" s="20"/>
       <c r="B22" t="s">
         <v>45</v>
       </c>
@@ -1097,7 +1127,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
+      <c r="A23" s="20"/>
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -1112,7 +1142,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="6" t="s">
         <v>9</v>
       </c>
@@ -1127,7 +1157,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="20" t="s">
         <v>53</v>
       </c>
       <c r="B26" t="s">
@@ -1144,7 +1174,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
+      <c r="A27" s="20"/>
       <c r="B27" t="s">
         <v>34</v>
       </c>
@@ -1159,7 +1189,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
+      <c r="A28" s="20"/>
       <c r="B28" t="s">
         <v>34</v>
       </c>
@@ -1174,7 +1204,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="6" t="s">
         <v>9</v>
       </c>
@@ -1189,7 +1219,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="20" t="s">
         <v>59</v>
       </c>
       <c r="B31" t="s">
@@ -1206,7 +1236,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
+      <c r="A32" s="20"/>
       <c r="B32" t="s">
         <v>34</v>
       </c>
@@ -1221,7 +1251,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
+      <c r="A33" s="20"/>
       <c r="B33" t="s">
         <v>34</v>
       </c>
@@ -1236,7 +1266,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="6" t="s">
         <v>9</v>
       </c>
@@ -1251,7 +1281,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="20" t="s">
         <v>63</v>
       </c>
       <c r="B36" t="s">
@@ -1268,7 +1298,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="18"/>
+      <c r="A37" s="20"/>
       <c r="B37" t="s">
         <v>45</v>
       </c>
@@ -1283,7 +1313,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
+      <c r="A38" s="20"/>
       <c r="B38" t="s">
         <v>34</v>
       </c>
@@ -1298,7 +1328,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="6" t="s">
         <v>9</v>
       </c>
@@ -1313,7 +1343,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B41" t="s">
@@ -1330,7 +1360,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
+      <c r="A42" s="19"/>
       <c r="B42" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
created read.md  & updated user stories excel sheet
</commit_message>
<xml_diff>
--- a/user_stories.xlsx
+++ b/user_stories.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="1260" yWindow="460" windowWidth="24340" windowHeight="14280" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1100" windowWidth="24340" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="84">
   <si>
     <t>Role 
 "As a"</t>
@@ -141,145 +141,153 @@
     <t xml:space="preserve">check the timer </t>
   </si>
   <si>
+    <t>land on round 2 page</t>
+  </si>
+  <si>
+    <t>am on round 2</t>
+  </si>
+  <si>
+    <t>click on the correct accessories/props for the character</t>
+  </si>
+  <si>
+    <t>drag the items on to the bare body character</t>
+  </si>
+  <si>
+    <t>drag the items on to the character</t>
+  </si>
+  <si>
+    <t>land on round 3 page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player chosen </t>
+  </si>
+  <si>
+    <t>am on round 3</t>
+  </si>
+  <si>
+    <t>scope through the multiple choice questions</t>
+  </si>
+  <si>
+    <t>land on round 4 page</t>
+  </si>
+  <si>
+    <t>am on round 4</t>
+  </si>
+  <si>
+    <t>drag the items on to the background</t>
+  </si>
+  <si>
+    <t>land on round 5 page</t>
+  </si>
+  <si>
+    <t>am on round 5</t>
+  </si>
+  <si>
+    <t>click on the background setting items for the character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click on the facial expressions </t>
+  </si>
+  <si>
+    <t>land on round 6 page</t>
+  </si>
+  <si>
+    <t>am on round 6</t>
+  </si>
+  <si>
+    <t>guess/click on the correct name of the character</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>land on the score board page</t>
+  </si>
+  <si>
+    <t>check individual scores</t>
+  </si>
+  <si>
+    <t>see how I did individually</t>
+  </si>
+  <si>
+    <t>check team scores</t>
+  </si>
+  <si>
+    <t>see how we did as a team</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>land on the answer page</t>
+  </si>
+  <si>
+    <t>check the solution and read the behind stories</t>
+  </si>
+  <si>
+    <t>see how ridiculous and ridiculously fun this game was!</t>
+  </si>
+  <si>
+    <t>check the score</t>
+  </si>
+  <si>
+    <t>check how we both are doing</t>
+  </si>
+  <si>
+    <t>am on round 13</t>
+  </si>
+  <si>
+    <t>am on round 16</t>
+  </si>
+  <si>
+    <t>Built</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Built (temp)</t>
+  </si>
+  <si>
     <t>Round 1
-: Attire</t>
-  </si>
-  <si>
-    <t>land on round 2 page</t>
-  </si>
-  <si>
-    <t>am on round 2</t>
-  </si>
-  <si>
-    <t>click on the correct accessories/props for the character</t>
-  </si>
-  <si>
-    <t>drag the items on to the bare body character</t>
-  </si>
-  <si>
-    <t>drag the items on to the character</t>
-  </si>
-  <si>
-    <t>keep track fo how much time I have left</t>
+Head</t>
   </si>
   <si>
     <t>Round 2
-: Acc/Prop</t>
-  </si>
-  <si>
-    <t>land on round 3 page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Player chosen </t>
-  </si>
-  <si>
-    <t>am on round 3</t>
-  </si>
-  <si>
-    <t>scope through the multiple choice questions</t>
+Face</t>
   </si>
   <si>
     <t>Round 3
-: Posture</t>
-  </si>
-  <si>
-    <t>click on the correct answers for the posture of the character</t>
-  </si>
-  <si>
-    <t>land on round 4 page</t>
-  </si>
-  <si>
-    <t>am on round 4</t>
-  </si>
-  <si>
-    <t>drag the items on to the background</t>
+Upper</t>
   </si>
   <si>
     <t>Round 4
-: Setting</t>
-  </si>
-  <si>
-    <t>land on round 5 page</t>
-  </si>
-  <si>
-    <t>am on round 5</t>
-  </si>
-  <si>
-    <t>click on the background setting items for the character</t>
-  </si>
-  <si>
-    <t xml:space="preserve">click on the facial expressions </t>
-  </si>
-  <si>
-    <t>drag the items on to the face</t>
+Lower</t>
   </si>
   <si>
     <t>Round 5
-: Mood</t>
-  </si>
-  <si>
-    <t>land on round 6 page</t>
-  </si>
-  <si>
-    <t>am on round 6</t>
-  </si>
-  <si>
-    <t>guess/click on the correct name of the character</t>
-  </si>
-  <si>
-    <t>Round 6
-: Name</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>land on the score board page</t>
-  </si>
-  <si>
-    <t>check individual scores</t>
-  </si>
-  <si>
-    <t>see how I did individually</t>
-  </si>
-  <si>
-    <t>check team scores</t>
-  </si>
-  <si>
-    <t>see how we did as a team</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t>land on the answer page</t>
-  </si>
-  <si>
-    <t>check the solution and read the behind stories</t>
-  </si>
-  <si>
-    <t>see how ridiculous and ridiculously fun this game was!</t>
-  </si>
-  <si>
-    <t>check the score</t>
-  </si>
-  <si>
-    <t>check how we both are doing</t>
-  </si>
-  <si>
-    <t>am on round 13</t>
-  </si>
-  <si>
-    <t>am on round 16</t>
-  </si>
-  <si>
-    <t>Built</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Built (temp)</t>
+Feet</t>
+  </si>
+  <si>
+    <t>Round 6 Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Click and append</t>
+  </si>
+  <si>
+    <t>click on the correct item character</t>
+  </si>
+  <si>
+    <t>drag the items on to the body</t>
+  </si>
+  <si>
+    <t>Not built</t>
+  </si>
+  <si>
+    <t>Random: No</t>
   </si>
 </sst>
 </file>
@@ -792,9 +800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,7 +812,7 @@
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
     <col min="4" max="4" width="46.83203125" customWidth="1"/>
     <col min="5" max="5" width="51.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="15" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="15" customWidth="1"/>
     <col min="7" max="7" width="8" style="15" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" style="15" customWidth="1"/>
   </cols>
@@ -852,10 +860,10 @@
         <v>15</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="H2" s="14"/>
     </row>
@@ -874,10 +882,10 @@
         <v>8</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -900,10 +908,10 @@
         <v>12</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -921,10 +929,10 @@
         <v>17</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -944,7 +952,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
@@ -964,15 +972,15 @@
         <v>24</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -985,6 +993,9 @@
       </c>
       <c r="E11" t="s">
         <v>31</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -999,7 +1010,13 @@
         <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1016,6 +1033,12 @@
       <c r="E13" t="s">
         <v>24</v>
       </c>
+      <c r="F13" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
@@ -1026,21 +1049,32 @@
         <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>66</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F15" s="15" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>30</v>
@@ -1048,61 +1082,82 @@
       <c r="E16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
       <c r="B17" t="s">
         <v>34</v>
       </c>
       <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
         <v>38</v>
       </c>
-      <c r="D17" t="s">
-        <v>39</v>
-      </c>
       <c r="E17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" t="s">
         <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
-        <v>48</v>
-      </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
         <v>30</v>
@@ -1110,61 +1165,82 @@
       <c r="E21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" t="s">
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
         <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>53</v>
-      </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D26" t="s">
         <v>30</v>
@@ -1172,61 +1248,82 @@
       <c r="E26" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
       <c r="B27" t="s">
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
       <c r="B28" t="s">
         <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
         <v>23</v>
       </c>
       <c r="E28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="20"/>
       <c r="B29" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -1234,61 +1331,82 @@
       <c r="E31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="20"/>
       <c r="B32" t="s">
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="20"/>
       <c r="B33" t="s">
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D33" t="s">
         <v>23</v>
       </c>
       <c r="E33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="20"/>
       <c r="B34" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
         <v>30</v>
@@ -1296,99 +1414,132 @@
       <c r="E36" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="20"/>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="20"/>
       <c r="B38" t="s">
         <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D38" t="s">
         <v>23</v>
       </c>
       <c r="E38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="20"/>
       <c r="B39" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E41" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="19"/>
       <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D42" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D44" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E44" t="s">
-        <v>73</v>
+        <v>64</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>